<commit_message>
finished axis control PCB design
</commit_message>
<xml_diff>
--- a/Electronics/axis_control_board/BOM/BOM.xlsx
+++ b/Electronics/axis_control_board/BOM/BOM.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ambadran717/Desktop/tmp_simacas/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ambadran717/Projects/SIMACAS/Electronics/axis_control_board/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3A76F5F0-0047-6A4D-8C95-2A5D12D5DBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34333869-E5CB-CD43-AFD5-282F1EBFEFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{04F109CC-B176-1341-9BDD-41DE0B865305}"/>
+    <workbookView xWindow="28800" yWindow="500" windowWidth="22040" windowHeight="14340" xr2:uid="{04F109CC-B176-1341-9BDD-41DE0B865305}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>No.</t>
   </si>
@@ -60,13 +60,76 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>STC8H8K64U1</t>
+  </si>
+  <si>
+    <t>nRF24l01</t>
+  </si>
+  <si>
+    <t>LD33v</t>
+  </si>
+  <si>
+    <t>lm7805</t>
+  </si>
+  <si>
+    <t>DRV8825</t>
+  </si>
+  <si>
+    <t>S8050</t>
+  </si>
+  <si>
+    <t>Resistors</t>
+  </si>
+  <si>
+    <t>1k, 220x2</t>
+  </si>
+  <si>
+    <t>Female Pin headers</t>
+  </si>
+  <si>
+    <t>JST female 2pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JST female 4pin </t>
+  </si>
+  <si>
+    <t>2 stepper motors output and one ultrasonic input/output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power in </t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Capacitor Electrolytic 220uF</t>
+  </si>
+  <si>
+    <t>Capacitor Electrolytic 22uF</t>
+  </si>
+  <si>
+    <t>Ceramic Capacitor</t>
+  </si>
+  <si>
+    <t>Ultrasonic Sensor</t>
+  </si>
+  <si>
+    <t>UGE</t>
+  </si>
+  <si>
+    <t>circuits-elec</t>
+  </si>
+  <si>
+    <t>PCB board</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,6 +145,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -91,7 +160,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -199,17 +268,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -406,11 +464,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -426,28 +534,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -782,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3335EA1C-5D69-B44C-90C9-DB5895DA7F87}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -795,7 +907,7 @@
     <col min="3" max="3" width="7.6640625" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="50" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -826,154 +938,347 @@
       <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="10">
-        <f t="shared" ref="E2:E10" si="0">C2*D2</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="12"/>
+      <c r="B2" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8">
+        <v>81</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="9">
+        <f t="shared" ref="E2:E12" si="0">C2*D2</f>
+        <v>81</v>
+      </c>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="12">
+      <c r="A3" s="11">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="15">
+      <c r="B3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="13">
+        <v>110</v>
+      </c>
+      <c r="D3" s="13">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F3" s="11"/>
-      <c r="G3" s="12"/>
+        <v>110</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="16"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="15">
+      <c r="B4" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="13">
+        <v>10</v>
+      </c>
+      <c r="D4" s="13">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="17"/>
-      <c r="G4" s="12"/>
+        <v>10</v>
+      </c>
+      <c r="F4" s="16"/>
+      <c r="G4" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="12">
+      <c r="A5" s="11">
         <v>4</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="15">
+      <c r="B5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="13">
+        <v>12</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="11"/>
-      <c r="G5" s="12"/>
+        <v>12</v>
+      </c>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="15">
+      <c r="B6" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="13">
+        <v>75</v>
+      </c>
+      <c r="D6" s="13">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="11"/>
-      <c r="G6" s="12"/>
+        <v>75</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="12">
+      <c r="A7" s="11">
         <v>6</v>
       </c>
-      <c r="B7" s="13"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="15">
+      <c r="B7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="13">
+        <v>140</v>
+      </c>
+      <c r="D7" s="13">
+        <v>2</v>
+      </c>
+      <c r="E7" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="12"/>
+        <v>280</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="13"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15">
+      <c r="B8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="13">
+        <v>3</v>
+      </c>
+      <c r="D8" s="13">
+        <v>1</v>
+      </c>
+      <c r="E8" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="11"/>
-      <c r="G8" s="12"/>
+        <v>3</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="12">
+      <c r="A9" s="11">
         <v>8</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15">
+      <c r="B9" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="13">
+        <v>5</v>
+      </c>
+      <c r="D9" s="13">
+        <v>3</v>
+      </c>
+      <c r="E9" s="14">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="11"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="7">
         <v>9</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15">
+      <c r="B10" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="13">
+        <v>2</v>
+      </c>
+      <c r="D10" s="13">
+        <v>1</v>
+      </c>
+      <c r="E10" s="14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="13">
+        <v>2</v>
+      </c>
+      <c r="D11" s="13">
+        <v>3</v>
+      </c>
+      <c r="E11" s="14">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="13">
+        <v>21</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F10" s="11"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="23"/>
-      <c r="B12" s="24" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="11">
+        <v>12</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="29">
+        <v>1</v>
+      </c>
+      <c r="D13" s="29">
+        <v>1</v>
+      </c>
+      <c r="E13" s="30"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="7"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="29">
+        <v>1</v>
+      </c>
+      <c r="D14" s="29">
+        <v>1</v>
+      </c>
+      <c r="E14" s="30"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" s="11">
+        <v>14</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="29">
+        <v>1</v>
+      </c>
+      <c r="D15" s="29">
+        <v>1</v>
+      </c>
+      <c r="E15" s="30"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="7"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="29">
+        <v>2</v>
+      </c>
+      <c r="D16" s="29">
+        <v>2</v>
+      </c>
+      <c r="E16" s="30"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="7"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="27"/>
+      <c r="B17" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="7"/>
+    </row>
+    <row r="18" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="17"/>
+      <c r="B18" s="18"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="22"/>
+      <c r="B19" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="1">
-        <f>SUM(E2:E11)</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="18"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="1">
+        <f>SUM(E2:E18)</f>
+        <v>594</v>
+      </c>
+      <c r="F19" s="22"/>
+      <c r="G19" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>